<commit_message>
updated hours and added a date row
</commit_message>
<xml_diff>
--- a/Documentation/EECS Project 2 Hours.xlsx
+++ b/Documentation/EECS Project 2 Hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/c354l536_home_ku_edu/Documents/Documents/GitHub/2/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewloaiza/Documents/KU/EECS_448/Projects/Project2_repo/eecs-448-Project-2/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_9CE44D60E2B816750CF7BD16D62528E350C244A7" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{68C7575F-F11F-4DD6-BE15-7062DF359D47}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB6FE37-7A0B-4141-9D74-87E2CA39BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="29800" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -289,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -343,11 +341,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,6 +360,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,18 +581,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -612,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -627,7 +626,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -660,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4"/>
       <c r="C9" s="7">
         <v>44460</v>
@@ -693,7 +692,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4"/>
       <c r="C10" s="7">
         <v>44465</v>
@@ -726,7 +725,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4"/>
       <c r="C11" s="7">
         <v>44469</v>
@@ -759,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4"/>
       <c r="C12" s="7">
         <v>44473</v>
@@ -792,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="4"/>
       <c r="C13" s="7">
         <v>44474</v>
@@ -825,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4"/>
       <c r="C14" s="7">
         <v>44475</v>
@@ -858,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="4"/>
       <c r="C15" s="9">
         <v>44477</v>
@@ -866,9 +865,13 @@
       <c r="D15" s="18">
         <v>2</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
+      <c r="E15" s="19">
+        <v>44478</v>
+      </c>
+      <c r="F15" s="20">
+        <v>4</v>
+      </c>
+      <c r="G15" s="19"/>
       <c r="H15" s="4"/>
       <c r="I15" s="9">
         <v>44477</v>
@@ -877,77 +880,72 @@
         <v>1</v>
       </c>
       <c r="K15" s="19"/>
-      <c r="L15" s="22"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="4"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="26"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4"/>
       <c r="I16" s="19">
         <v>44478</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="14">
         <v>2</v>
       </c>
       <c r="K16" s="19"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="28">
-        <f>SUM(D9:D16)</f>
+      <c r="D18" s="26">
+        <f>SUM(D9:D17)</f>
         <v>15</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28">
-        <f>SUM(F9:F15)</f>
-        <v>13.5</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28">
-        <f>SUM(H9:H15)</f>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26">
+        <f>SUM(F9:F17)</f>
+        <v>17.5</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26">
+        <f>SUM(H9:H17)</f>
         <v>14.5</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28">
-        <f>SUM(J9:J16)</f>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26">
+        <f>SUM(J9:J17)</f>
         <v>19</v>
       </c>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28">
+      <c r="K18" s="26"/>
+      <c r="L18" s="26">
         <f>SUM(L9:L15)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="4"/>
-      <c r="C19" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="29">
-        <f>D17+F17+H17+J17+L17</f>
-        <v>82</v>
-      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -957,77 +955,95 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="4"/>
+      <c r="C20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="27">
+        <f>D18+F18+H18+J18+L18</f>
+        <v>86</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>958</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="2">
-        <f>D19</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="2">
+        <f>D20</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="30">
-        <f>B24/B25</f>
-        <v>11.682926829268293</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B27" s="28">
+        <f>B25/B26</f>
+        <v>11.13953488372093</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="2">
         <v>200</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="29"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="30">
-        <f>B30/B26</f>
-        <v>29.95824634655532</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B33" s="28">
+        <f>B31/B27</f>
+        <v>31.419624217118997</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>